<commit_message>
update for manufacturability with npth vias
</commit_message>
<xml_diff>
--- a/Nákupní seznam.xlsx
+++ b/Nákupní seznam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marou\Projekty\Marek Coufal\GraviGon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751CEB96-A9E3-4FAC-AF10-68148006DF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E158FD8-61AC-4D56-80DB-6FCB508A2543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27540" yWindow="17750" windowWidth="22080" windowHeight="12970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14630" yWindow="0" windowWidth="14900" windowHeight="17770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>